<commit_message>
stopping point on Tuesday
</commit_message>
<xml_diff>
--- a/Data/ItemMap_20042014.xlsx
+++ b/Data/ItemMap_20042014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="8" r:id="rId1"/>
@@ -17,13 +17,16 @@
     <sheet name="Data Layout " sheetId="6" r:id="rId3"/>
     <sheet name="Renaming" sheetId="5" r:id="rId4"/>
     <sheet name="Time &amp; Age" sheetId="9" r:id="rId5"/>
-    <sheet name="Data Layout old" sheetId="1" state="hidden" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId6"/>
+    <sheet name="Data Layout old" sheetId="1" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Renaming!$A$2:$F$135</definedName>
+    <definedName name="comma">Sheet1!$K$1</definedName>
     <definedName name="dsSourceLabels" localSheetId="3">Renaming!$A$3:$C$135</definedName>
     <definedName name="q" localSheetId="4">'Time &amp; Age'!$U$5</definedName>
     <definedName name="q">'Data Layout '!$T$2</definedName>
+    <definedName name="quote">Sheet1!$J$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -97,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="440">
   <si>
     <t>x</t>
   </si>
@@ -1859,6 +1862,210 @@
   </si>
   <si>
     <t>Year of measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2234       1 1.  Roman Catholic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1854       2 2.  Baptist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     524       3 3.  Methodist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     406       4 4.  Lutheran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     150       5 5.  Presbyterian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     103       6 6.  Episcopal/Anglican</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     142       7 7.  United Church of Christ (or Congregationalist or </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     101       8 8.  Disciples of Christ (or the Christian Church)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      36       9 9.  Reform (or Reformed Church in America or Christian Reformed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     129      10 10.  Holiness (Nazarene, Wesleyan, Free Methodist)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     417      11 11.  Pentecostal (Assembly of God, Pentecostal Holiness)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     524      12 12.  Nondemonimational Christian (Bible Church)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     396      13 13.  Other Protestant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      12      14 14.  Jewish  -  Orthodox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      22      15 15.  Jewish  -  Conservative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      31      16 16.  Jewish  -  Reform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       7      17 17.  Jewish  -  Other Jewish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      92      18 18.  Mormon (all types of Latter Day Saints)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      12      19 19.  Eastern Orthodox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      15      20 20.  Unitarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      52      21 21.  Muslim (or Moslem or Islam)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      20      22 22.  Hindu/Buddhist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      17      23 23.  Native American Tribal Religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      29      26 25.  None, no religion - Atheist (confident there is no God)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     463      27 26.  None, no religion - Personal philosophy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       0      28 27.  Bah'ai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       0      30 28.  Greek, Roman, Norse, Etc. Mythology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       1      31 29.  Satanic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       8      32 30.  Wicca/Witchcraft/Magic/Pagan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       1      34 31.  Scientology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       2      35 32.  Other Eastern (Sikh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      24      24 33.  Other (SPECIFY)</t>
+  </si>
+  <si>
+    <t>Catholic</t>
+  </si>
+  <si>
+    <t>Baptist</t>
+  </si>
+  <si>
+    <t>Methodist</t>
+  </si>
+  <si>
+    <t>Lutheran</t>
+  </si>
+  <si>
+    <t>Presbyterian</t>
+  </si>
+  <si>
+    <t>Episcopal</t>
+  </si>
+  <si>
+    <t>C.Christ</t>
+  </si>
+  <si>
+    <t>D.Christ</t>
+  </si>
+  <si>
+    <t>Reformed</t>
+  </si>
+  <si>
+    <t>Holiness</t>
+  </si>
+  <si>
+    <t>Pentecostal</t>
+  </si>
+  <si>
+    <t>Non-Denom</t>
+  </si>
+  <si>
+    <t>OtherProt</t>
+  </si>
+  <si>
+    <t>JewishOrth</t>
+  </si>
+  <si>
+    <t>JewishCons</t>
+  </si>
+  <si>
+    <t>JewishRef</t>
+  </si>
+  <si>
+    <t>JewishOth</t>
+  </si>
+  <si>
+    <t>Mormon</t>
+  </si>
+  <si>
+    <t>EastOrth</t>
+  </si>
+  <si>
+    <t>Unitarian</t>
+  </si>
+  <si>
+    <t>Muslim</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>NATribal</t>
+  </si>
+  <si>
+    <t>Agnostic</t>
+  </si>
+  <si>
+    <t>Atheist</t>
+  </si>
+  <si>
+    <t>PersPhil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      90      25 24.  None, no religion - Agnostic (doesn't know if there is a God)</t>
+  </si>
+  <si>
+    <t>Bah'ai</t>
+  </si>
+  <si>
+    <t>Myth</t>
+  </si>
+  <si>
+    <t>Satanic</t>
+  </si>
+  <si>
+    <t>Witchcraft</t>
+  </si>
+  <si>
+    <t>Scientology</t>
+  </si>
+  <si>
+    <t>Sikh</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Baptic</t>
+  </si>
+  <si>
+    <t>Jewish</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2326,9 +2533,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2381,12 +2585,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="7">
     <dxf>
       <fill>
         <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
@@ -2499,535 +2707,6 @@
     </dxf>
     <dxf>
       <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="2"/>
         </patternFill>
@@ -3036,7 +2715,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -6186,8 +5865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A30"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7822,12 +7501,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="83" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="64" t="s">
         <v>368</v>
       </c>
@@ -10855,8 +10534,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.28515625" style="66" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="66" customWidth="1"/>
+    <col min="1" max="1" width="75.28515625" style="65" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="65" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="25" customWidth="1"/>
     <col min="4" max="4" width="5" style="22" customWidth="1"/>
     <col min="5" max="19" width="4.85546875" style="25" customWidth="1"/>
@@ -10865,14 +10544,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="73" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-      <c r="B4" s="67"/>
-      <c r="E4" s="73">
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
+      <c r="E4" s="72">
         <v>13</v>
       </c>
       <c r="F4" s="24">
@@ -10933,286 +10612,286 @@
     <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="69" t="s">
         <v>369</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="70">
         <v>1980</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76">
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75">
         <v>1997</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="75">
         <v>1998</v>
       </c>
-      <c r="K5" s="76">
+      <c r="K5" s="75">
         <v>1999</v>
       </c>
-      <c r="L5" s="76">
+      <c r="L5" s="75">
         <v>2000</v>
       </c>
-      <c r="M5" s="76">
+      <c r="M5" s="75">
         <v>2001</v>
       </c>
-      <c r="N5" s="76">
+      <c r="N5" s="75">
         <v>2002</v>
       </c>
-      <c r="O5" s="76">
+      <c r="O5" s="75">
         <v>2003</v>
       </c>
-      <c r="P5" s="76">
+      <c r="P5" s="75">
         <v>2004</v>
       </c>
-      <c r="Q5" s="76">
+      <c r="Q5" s="75">
         <v>2005</v>
       </c>
-      <c r="R5" s="76">
+      <c r="R5" s="75">
         <v>2006</v>
       </c>
-      <c r="S5" s="76">
+      <c r="S5" s="75">
         <v>2007</v>
       </c>
-      <c r="T5" s="76">
+      <c r="T5" s="75">
         <v>2008</v>
       </c>
-      <c r="U5" s="76">
+      <c r="U5" s="75">
         <v>2009</v>
       </c>
-      <c r="V5" s="76">
+      <c r="V5" s="75">
         <v>2010</v>
       </c>
-      <c r="W5" s="77">
+      <c r="W5" s="76">
         <v>2011</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
-      <c r="D6" s="72">
+      <c r="D6" s="71">
         <v>1981</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79">
+      <c r="E6" s="77"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78">
         <v>1997</v>
       </c>
-      <c r="I6" s="79">
+      <c r="I6" s="78">
         <v>1998</v>
       </c>
-      <c r="J6" s="79">
+      <c r="J6" s="78">
         <v>1999</v>
       </c>
-      <c r="K6" s="79">
+      <c r="K6" s="78">
         <v>2000</v>
       </c>
-      <c r="L6" s="79">
+      <c r="L6" s="78">
         <v>2001</v>
       </c>
-      <c r="M6" s="79">
+      <c r="M6" s="78">
         <v>2002</v>
       </c>
-      <c r="N6" s="79">
+      <c r="N6" s="78">
         <v>2003</v>
       </c>
-      <c r="O6" s="79">
+      <c r="O6" s="78">
         <v>2004</v>
       </c>
-      <c r="P6" s="79">
+      <c r="P6" s="78">
         <v>2005</v>
       </c>
-      <c r="Q6" s="79">
+      <c r="Q6" s="78">
         <v>2006</v>
       </c>
-      <c r="R6" s="79">
+      <c r="R6" s="78">
         <v>2007</v>
       </c>
-      <c r="S6" s="79">
+      <c r="S6" s="78">
         <v>2008</v>
       </c>
-      <c r="T6" s="79">
+      <c r="T6" s="78">
         <v>2009</v>
       </c>
-      <c r="U6" s="79">
+      <c r="U6" s="78">
         <v>2010</v>
       </c>
-      <c r="V6" s="79">
+      <c r="V6" s="78">
         <v>2011</v>
       </c>
-      <c r="W6" s="80"/>
+      <c r="W6" s="79"/>
     </row>
     <row r="7" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
-      <c r="D7" s="72">
+      <c r="D7" s="71">
         <v>1982</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79">
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78">
         <v>1997</v>
       </c>
-      <c r="H7" s="79">
+      <c r="H7" s="78">
         <v>1998</v>
       </c>
-      <c r="I7" s="79">
+      <c r="I7" s="78">
         <v>1999</v>
       </c>
-      <c r="J7" s="79">
+      <c r="J7" s="78">
         <v>2000</v>
       </c>
-      <c r="K7" s="79">
+      <c r="K7" s="78">
         <v>2001</v>
       </c>
-      <c r="L7" s="79">
+      <c r="L7" s="78">
         <v>2002</v>
       </c>
-      <c r="M7" s="79">
+      <c r="M7" s="78">
         <v>2003</v>
       </c>
-      <c r="N7" s="79">
+      <c r="N7" s="78">
         <v>2004</v>
       </c>
-      <c r="O7" s="79">
+      <c r="O7" s="78">
         <v>2005</v>
       </c>
-      <c r="P7" s="79">
+      <c r="P7" s="78">
         <v>2006</v>
       </c>
-      <c r="Q7" s="79">
+      <c r="Q7" s="78">
         <v>2007</v>
       </c>
-      <c r="R7" s="79">
+      <c r="R7" s="78">
         <v>2008</v>
       </c>
-      <c r="S7" s="79">
+      <c r="S7" s="78">
         <v>2009</v>
       </c>
-      <c r="T7" s="79">
+      <c r="T7" s="78">
         <v>2010</v>
       </c>
-      <c r="U7" s="79">
+      <c r="U7" s="78">
         <v>2011</v>
       </c>
-      <c r="V7" s="79"/>
-      <c r="W7" s="80"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="79"/>
     </row>
     <row r="8" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
-      <c r="D8" s="72">
+      <c r="D8" s="71">
         <v>1983</v>
       </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79">
+      <c r="E8" s="77"/>
+      <c r="F8" s="78">
         <v>1997</v>
       </c>
-      <c r="G8" s="79">
+      <c r="G8" s="78">
         <v>1998</v>
       </c>
-      <c r="H8" s="79">
+      <c r="H8" s="78">
         <v>1999</v>
       </c>
-      <c r="I8" s="79">
+      <c r="I8" s="78">
         <v>2000</v>
       </c>
-      <c r="J8" s="79">
+      <c r="J8" s="78">
         <v>2001</v>
       </c>
-      <c r="K8" s="79">
+      <c r="K8" s="78">
         <v>2002</v>
       </c>
-      <c r="L8" s="79">
+      <c r="L8" s="78">
         <v>2003</v>
       </c>
-      <c r="M8" s="79">
+      <c r="M8" s="78">
         <v>2004</v>
       </c>
-      <c r="N8" s="79">
+      <c r="N8" s="78">
         <v>2005</v>
       </c>
-      <c r="O8" s="79">
+      <c r="O8" s="78">
         <v>2006</v>
       </c>
-      <c r="P8" s="79">
+      <c r="P8" s="78">
         <v>2007</v>
       </c>
-      <c r="Q8" s="79">
+      <c r="Q8" s="78">
         <v>2008</v>
       </c>
-      <c r="R8" s="79">
+      <c r="R8" s="78">
         <v>2009</v>
       </c>
-      <c r="S8" s="79">
+      <c r="S8" s="78">
         <v>2010</v>
       </c>
-      <c r="T8" s="79">
+      <c r="T8" s="78">
         <v>2011</v>
       </c>
-      <c r="U8" s="79"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="80"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="79"/>
     </row>
     <row r="9" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="26"/>
-      <c r="D9" s="72">
+      <c r="D9" s="71">
         <v>1984</v>
       </c>
-      <c r="E9" s="81">
+      <c r="E9" s="80">
         <v>1997</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="81">
         <v>1998</v>
       </c>
-      <c r="G9" s="82">
+      <c r="G9" s="81">
         <v>1999</v>
       </c>
-      <c r="H9" s="82">
+      <c r="H9" s="81">
         <v>2000</v>
       </c>
-      <c r="I9" s="82">
+      <c r="I9" s="81">
         <v>2001</v>
       </c>
-      <c r="J9" s="82">
+      <c r="J9" s="81">
         <v>2002</v>
       </c>
-      <c r="K9" s="82">
+      <c r="K9" s="81">
         <v>2003</v>
       </c>
-      <c r="L9" s="82">
+      <c r="L9" s="81">
         <v>2004</v>
       </c>
-      <c r="M9" s="82">
+      <c r="M9" s="81">
         <v>2005</v>
       </c>
-      <c r="N9" s="82">
+      <c r="N9" s="81">
         <v>2006</v>
       </c>
-      <c r="O9" s="82">
+      <c r="O9" s="81">
         <v>2007</v>
       </c>
-      <c r="P9" s="82">
+      <c r="P9" s="81">
         <v>2008</v>
       </c>
-      <c r="Q9" s="82">
+      <c r="Q9" s="81">
         <v>2009</v>
       </c>
-      <c r="R9" s="82">
+      <c r="R9" s="81">
         <v>2010</v>
       </c>
-      <c r="S9" s="82">
+      <c r="S9" s="81">
         <v>2011</v>
       </c>
-      <c r="T9" s="82"/>
-      <c r="U9" s="82"/>
-      <c r="V9" s="82"/>
-      <c r="W9" s="83"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="82"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" s="55"/>
@@ -11237,89 +10916,89 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J11" s="69"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
-      <c r="J12" s="69"/>
+      <c r="J12" s="68"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
-      <c r="B13" s="68"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="67"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="N14" s="69"/>
+      <c r="N14" s="68"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N18" s="69"/>
+      <c r="N18" s="68"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="68"/>
-      <c r="N19" s="69"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
+      <c r="N19" s="68"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
-      <c r="N20" s="69"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="N20" s="68"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="69"/>
+      <c r="N21" s="68"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="68"/>
-      <c r="B22" s="68"/>
-      <c r="N22" s="69"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="N22" s="68"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N23" s="69"/>
+      <c r="N23" s="68"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O25" s="69"/>
+      <c r="O25" s="68"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="68"/>
-      <c r="B26" s="68"/>
-      <c r="O26" s="69"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+      <c r="O26" s="68"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="O27" s="69"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="O27" s="68"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="68"/>
-      <c r="O28" s="69"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="O28" s="68"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="68"/>
-      <c r="B33" s="68"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
-      <c r="B34" s="68"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="67"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="68"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="67"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="68"/>
-      <c r="B36" s="68"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E25:S28 E14:S14 E11:S12 O18:S22 E18:M22 N18:N23">
@@ -11339,6 +11018,924 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O2:O34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J1" s="84" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" t="str">
+        <f>MID(A2,21,40)</f>
+        <v>Roman Catholic</v>
+      </c>
+      <c r="G2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I2" t="s">
+        <v>404</v>
+      </c>
+      <c r="K2" t="str">
+        <f>LEFT(A2,9)</f>
+        <v xml:space="preserve">   2234  </v>
+      </c>
+      <c r="M2" t="str">
+        <f>CONCATENATE(quote,G2,quote,comma)</f>
+        <v>"Catholic",</v>
+      </c>
+      <c r="O2" t="str">
+        <f>CONCATENATE(quote,I2,quote,comma)</f>
+        <v>"Catholic",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B34" si="0">MID(A3,21,40)</f>
+        <v xml:space="preserve"> Baptist</v>
+      </c>
+      <c r="G3" t="s">
+        <v>405</v>
+      </c>
+      <c r="I3" t="s">
+        <v>438</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K34" si="1">LEFT(A3,9)</f>
+        <v xml:space="preserve">    1854 </v>
+      </c>
+      <c r="M3" t="str">
+        <f>CONCATENATE(quote,G3,quote,comma)</f>
+        <v>"Baptist",</v>
+      </c>
+      <c r="O3" t="str">
+        <f>CONCATENATE(quote,I3,quote,comma)</f>
+        <v>"Baptic",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Methodist</v>
+      </c>
+      <c r="G4" t="s">
+        <v>406</v>
+      </c>
+      <c r="I4" t="s">
+        <v>406</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     524 </v>
+      </c>
+      <c r="M4" t="str">
+        <f>CONCATENATE(quote,G4,quote,comma)</f>
+        <v>"Methodist",</v>
+      </c>
+      <c r="O4" t="str">
+        <f>CONCATENATE(quote,I4,quote,comma)</f>
+        <v>"Methodist",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Lutheran</v>
+      </c>
+      <c r="G5" t="s">
+        <v>407</v>
+      </c>
+      <c r="I5" t="s">
+        <v>407</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     406 </v>
+      </c>
+      <c r="M5" t="str">
+        <f>CONCATENATE(quote,G5,quote,comma)</f>
+        <v>"Lutheran",</v>
+      </c>
+      <c r="O5" t="str">
+        <f>CONCATENATE(quote,I5,quote,comma)</f>
+        <v>"Lutheran",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Presbyterian</v>
+      </c>
+      <c r="G6" t="s">
+        <v>408</v>
+      </c>
+      <c r="I6" t="s">
+        <v>408</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     150 </v>
+      </c>
+      <c r="M6" t="str">
+        <f>CONCATENATE(quote,G6,quote,comma)</f>
+        <v>"Presbyterian",</v>
+      </c>
+      <c r="O6" t="str">
+        <f>CONCATENATE(quote,I6,quote,comma)</f>
+        <v>"Presbyterian",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Episcopal/Anglican</v>
+      </c>
+      <c r="G7" t="s">
+        <v>409</v>
+      </c>
+      <c r="I7" t="s">
+        <v>409</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     103 </v>
+      </c>
+      <c r="M7" t="str">
+        <f>CONCATENATE(quote,G7,quote,comma)</f>
+        <v>"Episcopal",</v>
+      </c>
+      <c r="O7" t="str">
+        <f>CONCATENATE(quote,I7,quote,comma)</f>
+        <v>"Episcopal",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> United Church of Christ (or Congregatio</v>
+      </c>
+      <c r="G8" t="s">
+        <v>410</v>
+      </c>
+      <c r="I8" t="s">
+        <v>416</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     142 </v>
+      </c>
+      <c r="M8" t="str">
+        <f>CONCATENATE(quote,G8,quote,comma)</f>
+        <v>"C.Christ",</v>
+      </c>
+      <c r="O8" t="str">
+        <f>CONCATENATE(quote,I8,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Disciples of Christ (or the Christian C</v>
+      </c>
+      <c r="G9" t="s">
+        <v>411</v>
+      </c>
+      <c r="I9" t="s">
+        <v>416</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     101 </v>
+      </c>
+      <c r="M9" t="str">
+        <f>CONCATENATE(quote,G9,quote,comma)</f>
+        <v>"D.Christ",</v>
+      </c>
+      <c r="O9" t="str">
+        <f>CONCATENATE(quote,I9,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>380</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Reform (or Reformed Church in America o</v>
+      </c>
+      <c r="G10" t="s">
+        <v>412</v>
+      </c>
+      <c r="I10" t="s">
+        <v>416</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      36 </v>
+      </c>
+      <c r="M10" t="str">
+        <f>CONCATENATE(quote,G10,quote,comma)</f>
+        <v>"Reformed",</v>
+      </c>
+      <c r="O10" t="str">
+        <f>CONCATENATE(quote,I10,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>381</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Holiness (Nazarene, Wesleyan, Free Met</v>
+      </c>
+      <c r="G11" t="s">
+        <v>413</v>
+      </c>
+      <c r="I11" t="s">
+        <v>416</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     129 </v>
+      </c>
+      <c r="M11" t="str">
+        <f>CONCATENATE(quote,G11,quote,comma)</f>
+        <v>"Holiness",</v>
+      </c>
+      <c r="O11" t="str">
+        <f>CONCATENATE(quote,I11,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Pentecostal (Assembly of God, Pentecos</v>
+      </c>
+      <c r="G12" t="s">
+        <v>414</v>
+      </c>
+      <c r="I12" t="s">
+        <v>414</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     417 </v>
+      </c>
+      <c r="M12" t="str">
+        <f>CONCATENATE(quote,G12,quote,comma)</f>
+        <v>"Pentecostal",</v>
+      </c>
+      <c r="O12" t="str">
+        <f>CONCATENATE(quote,I12,quote,comma)</f>
+        <v>"Pentecostal",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Nondemonimational Christian (Bible Chu</v>
+      </c>
+      <c r="G13" t="s">
+        <v>415</v>
+      </c>
+      <c r="I13" t="s">
+        <v>415</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     524 </v>
+      </c>
+      <c r="M13" t="str">
+        <f>CONCATENATE(quote,G13,quote,comma)</f>
+        <v>"Non-Denom",</v>
+      </c>
+      <c r="O13" t="str">
+        <f>CONCATENATE(quote,I13,quote,comma)</f>
+        <v>"Non-Denom",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>384</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Other Protestant</v>
+      </c>
+      <c r="G14" t="s">
+        <v>416</v>
+      </c>
+      <c r="I14" t="s">
+        <v>416</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     396 </v>
+      </c>
+      <c r="M14" t="str">
+        <f>CONCATENATE(quote,G14,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+      <c r="O14" t="str">
+        <f>CONCATENATE(quote,I14,quote,comma)</f>
+        <v>"OtherProt",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>385</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Jewish  -  Orthodox</v>
+      </c>
+      <c r="G15" t="s">
+        <v>417</v>
+      </c>
+      <c r="I15" t="s">
+        <v>439</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      12 </v>
+      </c>
+      <c r="M15" t="str">
+        <f>CONCATENATE(quote,G15,quote,comma)</f>
+        <v>"JewishOrth",</v>
+      </c>
+      <c r="O15" t="str">
+        <f>CONCATENATE(quote,I15,quote,comma)</f>
+        <v>"Jewish",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>386</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Jewish  -  Conservative</v>
+      </c>
+      <c r="G16" t="s">
+        <v>418</v>
+      </c>
+      <c r="I16" t="s">
+        <v>439</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      22 </v>
+      </c>
+      <c r="M16" t="str">
+        <f>CONCATENATE(quote,G16,quote,comma)</f>
+        <v>"JewishCons",</v>
+      </c>
+      <c r="O16" t="str">
+        <f>CONCATENATE(quote,I16,quote,comma)</f>
+        <v>"Jewish",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>387</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Jewish  -  Reform</v>
+      </c>
+      <c r="G17" t="s">
+        <v>419</v>
+      </c>
+      <c r="I17" t="s">
+        <v>439</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      31 </v>
+      </c>
+      <c r="M17" t="str">
+        <f>CONCATENATE(quote,G17,quote,comma)</f>
+        <v>"JewishRef",</v>
+      </c>
+      <c r="O17" t="str">
+        <f>CONCATENATE(quote,I17,quote,comma)</f>
+        <v>"Jewish",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>388</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Jewish  -  Other Jewish</v>
+      </c>
+      <c r="G18" t="s">
+        <v>420</v>
+      </c>
+      <c r="I18" t="s">
+        <v>439</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       7 </v>
+      </c>
+      <c r="M18" t="str">
+        <f>CONCATENATE(quote,G18,quote,comma)</f>
+        <v>"JewishOth",</v>
+      </c>
+      <c r="O18" t="str">
+        <f>CONCATENATE(quote,I18,quote,comma)</f>
+        <v>"Jewish",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>389</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Mormon (all types of Latter Day Saints</v>
+      </c>
+      <c r="G19" t="s">
+        <v>421</v>
+      </c>
+      <c r="I19" t="s">
+        <v>421</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      92 </v>
+      </c>
+      <c r="M19" t="str">
+        <f>CONCATENATE(quote,G19,quote,comma)</f>
+        <v>"Mormon",</v>
+      </c>
+      <c r="O19" t="str">
+        <f>CONCATENATE(quote,I19,quote,comma)</f>
+        <v>"Mormon",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>390</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Eastern Orthodox</v>
+      </c>
+      <c r="G20" t="s">
+        <v>422</v>
+      </c>
+      <c r="I20" t="s">
+        <v>422</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      12 </v>
+      </c>
+      <c r="M20" t="str">
+        <f>CONCATENATE(quote,G20,quote,comma)</f>
+        <v>"EastOrth",</v>
+      </c>
+      <c r="O20" t="str">
+        <f>CONCATENATE(quote,I20,quote,comma)</f>
+        <v>"EastOrth",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>391</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Unitarian</v>
+      </c>
+      <c r="G21" t="s">
+        <v>423</v>
+      </c>
+      <c r="I21" t="s">
+        <v>423</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      15 </v>
+      </c>
+      <c r="M21" t="str">
+        <f>CONCATENATE(quote,G21,quote,comma)</f>
+        <v>"Unitarian",</v>
+      </c>
+      <c r="O21" t="str">
+        <f>CONCATENATE(quote,I21,quote,comma)</f>
+        <v>"Unitarian",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Muslim (or Moslem or Islam)</v>
+      </c>
+      <c r="G22" t="s">
+        <v>424</v>
+      </c>
+      <c r="I22" t="s">
+        <v>424</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      52 </v>
+      </c>
+      <c r="M22" t="str">
+        <f>CONCATENATE(quote,G22,quote,comma)</f>
+        <v>"Muslim",</v>
+      </c>
+      <c r="O22" t="str">
+        <f>CONCATENATE(quote,I22,quote,comma)</f>
+        <v>"Muslim",</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>393</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Hindu/Buddhist</v>
+      </c>
+      <c r="G23" t="s">
+        <v>425</v>
+      </c>
+      <c r="I23" t="s">
+        <v>437</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      20 </v>
+      </c>
+      <c r="M23" t="str">
+        <f>CONCATENATE(quote,G23,quote,comma)</f>
+        <v>"Hindu",</v>
+      </c>
+      <c r="O23" t="str">
+        <f>CONCATENATE(quote,I23,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>394</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Native American Tribal Religion</v>
+      </c>
+      <c r="G24" t="s">
+        <v>426</v>
+      </c>
+      <c r="I24" t="s">
+        <v>437</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      17 </v>
+      </c>
+      <c r="M24" t="str">
+        <f>CONCATENATE(quote,G24,quote,comma)</f>
+        <v>"NATribal",</v>
+      </c>
+      <c r="O24" t="str">
+        <f>CONCATENATE(quote,I24,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>430</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  None, no religion - Agnostic (doesn't </v>
+      </c>
+      <c r="G25" t="s">
+        <v>427</v>
+      </c>
+      <c r="I25" t="s">
+        <v>437</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      90 </v>
+      </c>
+      <c r="M25" t="str">
+        <f>CONCATENATE(quote,G25,quote,comma)</f>
+        <v>"Agnostic",</v>
+      </c>
+      <c r="O25" t="str">
+        <f>CONCATENATE(quote,I25,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B26" t="str">
+        <f>MID(A26,21,40)</f>
+        <v xml:space="preserve">  None, no religion - Atheist (confident</v>
+      </c>
+      <c r="G26" t="s">
+        <v>428</v>
+      </c>
+      <c r="I26" t="s">
+        <v>437</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      29 </v>
+      </c>
+      <c r="M26" t="str">
+        <f>CONCATENATE(quote,G26,quote,comma)</f>
+        <v>"Atheist",</v>
+      </c>
+      <c r="O26" t="str">
+        <f>CONCATENATE(quote,I26,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  None, no religion - Personal philosoph</v>
+      </c>
+      <c r="G27" t="s">
+        <v>429</v>
+      </c>
+      <c r="I27" t="s">
+        <v>437</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">     463 </v>
+      </c>
+      <c r="M27" t="str">
+        <f>CONCATENATE(quote,G27,quote,comma)</f>
+        <v>"PersPhil",</v>
+      </c>
+      <c r="O27" t="str">
+        <f>CONCATENATE(quote,I27,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>397</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Bah'ai</v>
+      </c>
+      <c r="G28" t="s">
+        <v>431</v>
+      </c>
+      <c r="I28" t="s">
+        <v>437</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       0 </v>
+      </c>
+      <c r="M28" t="str">
+        <f>CONCATENATE(quote,G28,quote,comma)</f>
+        <v>"Bah'ai",</v>
+      </c>
+      <c r="O28" t="str">
+        <f>CONCATENATE(quote,I28,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>398</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Greek, Roman, Norse, Etc. Mythology</v>
+      </c>
+      <c r="G29" t="s">
+        <v>432</v>
+      </c>
+      <c r="I29" t="s">
+        <v>437</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       0 </v>
+      </c>
+      <c r="M29" t="str">
+        <f>CONCATENATE(quote,G29,quote,comma)</f>
+        <v>"Myth",</v>
+      </c>
+      <c r="O29" t="str">
+        <f>CONCATENATE(quote,I29,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>399</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Satanic</v>
+      </c>
+      <c r="G30" t="s">
+        <v>433</v>
+      </c>
+      <c r="I30" t="s">
+        <v>437</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       1 </v>
+      </c>
+      <c r="M30" t="str">
+        <f>CONCATENATE(quote,G30,quote,comma)</f>
+        <v>"Satanic",</v>
+      </c>
+      <c r="O30" t="str">
+        <f>CONCATENATE(quote,I30,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>400</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Wicca/Witchcraft/Magic/Pagan</v>
+      </c>
+      <c r="G31" t="s">
+        <v>434</v>
+      </c>
+      <c r="I31" t="s">
+        <v>437</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       8 </v>
+      </c>
+      <c r="M31" t="str">
+        <f>CONCATENATE(quote,G31,quote,comma)</f>
+        <v>"Witchcraft",</v>
+      </c>
+      <c r="O31" t="str">
+        <f>CONCATENATE(quote,I31,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>401</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Scientology</v>
+      </c>
+      <c r="G32" t="s">
+        <v>435</v>
+      </c>
+      <c r="I32" t="s">
+        <v>437</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       1 </v>
+      </c>
+      <c r="M32" t="str">
+        <f>CONCATENATE(quote,G32,quote,comma)</f>
+        <v>"Scientology",</v>
+      </c>
+      <c r="O32" t="str">
+        <f>CONCATENATE(quote,I32,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>402</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Other Eastern (Sikh)</v>
+      </c>
+      <c r="G33" t="s">
+        <v>436</v>
+      </c>
+      <c r="I33" t="s">
+        <v>436</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">       2 </v>
+      </c>
+      <c r="M33" t="str">
+        <f>CONCATENATE(quote,G33,quote,comma)</f>
+        <v>"Sikh",</v>
+      </c>
+      <c r="O33" t="str">
+        <f>CONCATENATE(quote,I33,quote,comma)</f>
+        <v>"Sikh",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>403</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  Other (SPECIFY)</v>
+      </c>
+      <c r="G34" t="s">
+        <v>437</v>
+      </c>
+      <c r="I34" t="s">
+        <v>437</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">      24 </v>
+      </c>
+      <c r="M34" t="str">
+        <f>CONCATENATE(quote,G34,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+      <c r="O34" t="str">
+        <f>CONCATENATE(quote,I34,quote,comma)</f>
+        <v>"Other",</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X58"/>
   <sheetViews>

</xml_diff>

<commit_message>
transposed age by cohort thumbs
</commit_message>
<xml_diff>
--- a/Data/ItemMap_20042014.xlsx
+++ b/Data/ItemMap_20042014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="5"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="8" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="441">
   <si>
     <t>x</t>
   </si>
@@ -2066,6 +2066,9 @@
   </si>
   <si>
     <t>Jewish</t>
+  </si>
+  <si>
+    <t>Age years</t>
   </si>
 </sst>
 </file>
@@ -2359,7 +2362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2585,16 +2588,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
     <dxf>
       <fill>
         <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
@@ -2632,6 +2647,30 @@
           <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2707,6 +2746,54 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="2"/>
         </patternFill>
@@ -2715,7 +2802,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -7465,12 +7552,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D54:R57 D34:R34 D43:R43 B11:C12 B14:C14 D40:R41 N47:R51 D47:L51 M47:M52">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:R30">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7501,12 +7588,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
       <c r="E1" s="64" t="s">
         <v>368</v>
       </c>
@@ -10526,10 +10613,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:W36"/>
+  <dimension ref="A3:AF36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="N3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10540,15 +10627,19 @@
     <col min="4" max="4" width="5" style="22" customWidth="1"/>
     <col min="5" max="19" width="4.85546875" style="25" customWidth="1"/>
     <col min="20" max="23" width="4.85546875" style="55" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="55"/>
+    <col min="24" max="24" width="9.140625" style="55"/>
+    <col min="25" max="25" width="5.140625" style="55" customWidth="1"/>
+    <col min="26" max="27" width="4.85546875" style="55" customWidth="1"/>
+    <col min="28" max="32" width="5.85546875" style="55" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E3" s="73" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
       <c r="B4" s="66"/>
       <c r="E4" s="72">
@@ -10608,8 +10699,11 @@
       <c r="W4" s="24">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB4" s="73" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="69" t="s">
@@ -10667,8 +10761,23 @@
       <c r="W5" s="76">
         <v>2011</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB5" s="87">
+        <v>1980</v>
+      </c>
+      <c r="AC5" s="88">
+        <v>1981</v>
+      </c>
+      <c r="AD5" s="88">
+        <v>1982</v>
+      </c>
+      <c r="AE5" s="88">
+        <v>1983</v>
+      </c>
+      <c r="AF5" s="88">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
       <c r="D6" s="71">
@@ -10723,8 +10832,22 @@
         <v>2011</v>
       </c>
       <c r="W6" s="79"/>
-    </row>
-    <row r="7" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y6" s="53"/>
+      <c r="Z6" s="69" t="s">
+        <v>440</v>
+      </c>
+      <c r="AA6" s="86">
+        <v>13</v>
+      </c>
+      <c r="AB6" s="74"/>
+      <c r="AC6" s="75"/>
+      <c r="AD6" s="75"/>
+      <c r="AE6" s="75"/>
+      <c r="AF6" s="76">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="D7" s="71">
@@ -10779,8 +10902,20 @@
       </c>
       <c r="V7" s="78"/>
       <c r="W7" s="79"/>
-    </row>
-    <row r="8" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA7" s="85">
+        <v>14</v>
+      </c>
+      <c r="AB7" s="77"/>
+      <c r="AC7" s="78"/>
+      <c r="AD7" s="78"/>
+      <c r="AE7" s="78">
+        <v>1997</v>
+      </c>
+      <c r="AF7" s="79">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="D8" s="71">
@@ -10835,8 +10970,22 @@
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
       <c r="W8" s="79"/>
-    </row>
-    <row r="9" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA8" s="85">
+        <v>15</v>
+      </c>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="78"/>
+      <c r="AD8" s="78">
+        <v>1997</v>
+      </c>
+      <c r="AE8" s="78">
+        <v>1998</v>
+      </c>
+      <c r="AF8" s="79">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="26"/>
@@ -10892,8 +11041,24 @@
       <c r="U9" s="81"/>
       <c r="V9" s="81"/>
       <c r="W9" s="82"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA9" s="85">
+        <v>16</v>
+      </c>
+      <c r="AB9" s="77"/>
+      <c r="AC9" s="78">
+        <v>1997</v>
+      </c>
+      <c r="AD9" s="78">
+        <v>1998</v>
+      </c>
+      <c r="AE9" s="78">
+        <v>1999</v>
+      </c>
+      <c r="AF9" s="79">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
@@ -10914,73 +11079,331 @@
       <c r="W10" s="22" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA10" s="85">
+        <v>17</v>
+      </c>
+      <c r="AB10" s="77">
+        <v>1997</v>
+      </c>
+      <c r="AC10" s="78">
+        <v>1998</v>
+      </c>
+      <c r="AD10" s="78">
+        <v>1999</v>
+      </c>
+      <c r="AE10" s="78">
+        <v>2000</v>
+      </c>
+      <c r="AF10" s="79">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="J11" s="68"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA11" s="85">
+        <v>18</v>
+      </c>
+      <c r="AB11" s="77">
+        <v>1998</v>
+      </c>
+      <c r="AC11" s="78">
+        <v>1999</v>
+      </c>
+      <c r="AD11" s="78">
+        <v>2000</v>
+      </c>
+      <c r="AE11" s="78">
+        <v>2001</v>
+      </c>
+      <c r="AF11" s="79">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
       <c r="J12" s="68"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA12" s="85">
+        <v>19</v>
+      </c>
+      <c r="AB12" s="77">
+        <v>1999</v>
+      </c>
+      <c r="AC12" s="78">
+        <v>2000</v>
+      </c>
+      <c r="AD12" s="78">
+        <v>2001</v>
+      </c>
+      <c r="AE12" s="78">
+        <v>2002</v>
+      </c>
+      <c r="AF12" s="79">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
       <c r="B13" s="67"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA13" s="85">
+        <v>20</v>
+      </c>
+      <c r="AB13" s="77">
+        <v>2000</v>
+      </c>
+      <c r="AC13" s="78">
+        <v>2001</v>
+      </c>
+      <c r="AD13" s="78">
+        <v>2002</v>
+      </c>
+      <c r="AE13" s="78">
+        <v>2003</v>
+      </c>
+      <c r="AF13" s="79">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N14" s="68"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA14" s="85">
+        <v>21</v>
+      </c>
+      <c r="AB14" s="77">
+        <v>2001</v>
+      </c>
+      <c r="AC14" s="78">
+        <v>2002</v>
+      </c>
+      <c r="AD14" s="78">
+        <v>2003</v>
+      </c>
+      <c r="AE14" s="78">
+        <v>2004</v>
+      </c>
+      <c r="AF14" s="79">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA15" s="85">
+        <v>22</v>
+      </c>
+      <c r="AB15" s="77">
+        <v>2002</v>
+      </c>
+      <c r="AC15" s="78">
+        <v>2003</v>
+      </c>
+      <c r="AD15" s="78">
+        <v>2004</v>
+      </c>
+      <c r="AE15" s="78">
+        <v>2005</v>
+      </c>
+      <c r="AF15" s="79">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA16" s="85">
+        <v>23</v>
+      </c>
+      <c r="AB16" s="77">
+        <v>2003</v>
+      </c>
+      <c r="AC16" s="78">
+        <v>2004</v>
+      </c>
+      <c r="AD16" s="78">
+        <v>2005</v>
+      </c>
+      <c r="AE16" s="78">
+        <v>2006</v>
+      </c>
+      <c r="AF16" s="79">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA17" s="85">
+        <v>24</v>
+      </c>
+      <c r="AB17" s="77">
+        <v>2004</v>
+      </c>
+      <c r="AC17" s="78">
+        <v>2005</v>
+      </c>
+      <c r="AD17" s="78">
+        <v>2006</v>
+      </c>
+      <c r="AE17" s="78">
+        <v>2007</v>
+      </c>
+      <c r="AF17" s="79">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N18" s="68"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA18" s="85">
+        <v>25</v>
+      </c>
+      <c r="AB18" s="77">
+        <v>2005</v>
+      </c>
+      <c r="AC18" s="78">
+        <v>2006</v>
+      </c>
+      <c r="AD18" s="78">
+        <v>2007</v>
+      </c>
+      <c r="AE18" s="78">
+        <v>2008</v>
+      </c>
+      <c r="AF18" s="79">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="67"/>
       <c r="B19" s="67"/>
       <c r="N19" s="68"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA19" s="85">
+        <v>26</v>
+      </c>
+      <c r="AB19" s="77">
+        <v>2006</v>
+      </c>
+      <c r="AC19" s="78">
+        <v>2007</v>
+      </c>
+      <c r="AD19" s="78">
+        <v>2008</v>
+      </c>
+      <c r="AE19" s="78">
+        <v>2009</v>
+      </c>
+      <c r="AF19" s="79">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="67"/>
       <c r="B20" s="67"/>
       <c r="N20" s="68"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA20" s="85">
+        <v>27</v>
+      </c>
+      <c r="AB20" s="77">
+        <v>2007</v>
+      </c>
+      <c r="AC20" s="78">
+        <v>2008</v>
+      </c>
+      <c r="AD20" s="78">
+        <v>2009</v>
+      </c>
+      <c r="AE20" s="78">
+        <v>2010</v>
+      </c>
+      <c r="AF20" s="79">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N21" s="68"/>
-    </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA21" s="85">
+        <v>28</v>
+      </c>
+      <c r="AB21" s="77">
+        <v>2008</v>
+      </c>
+      <c r="AC21" s="78">
+        <v>2009</v>
+      </c>
+      <c r="AD21" s="78">
+        <v>2010</v>
+      </c>
+      <c r="AE21" s="78">
+        <v>2011</v>
+      </c>
+      <c r="AF21" s="79"/>
+    </row>
+    <row r="22" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67"/>
       <c r="B22" s="67"/>
       <c r="N22" s="68"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA22" s="85">
+        <v>29</v>
+      </c>
+      <c r="AB22" s="77">
+        <v>2009</v>
+      </c>
+      <c r="AC22" s="78">
+        <v>2010</v>
+      </c>
+      <c r="AD22" s="78">
+        <v>2011</v>
+      </c>
+      <c r="AE22" s="78"/>
+      <c r="AF22" s="79"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N23" s="68"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="AA23" s="85">
+        <v>30</v>
+      </c>
+      <c r="AB23" s="77">
+        <v>2010</v>
+      </c>
+      <c r="AC23" s="78">
+        <v>2011</v>
+      </c>
+      <c r="AD23" s="78"/>
+      <c r="AE23" s="78"/>
+      <c r="AF23" s="79"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA24" s="85">
+        <v>31</v>
+      </c>
+      <c r="AB24" s="80">
+        <v>2011</v>
+      </c>
+      <c r="AC24" s="81"/>
+      <c r="AD24" s="81"/>
+      <c r="AE24" s="81"/>
+      <c r="AF24" s="82"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="O25" s="68"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="67"/>
       <c r="B26" s="67"/>
       <c r="O26" s="68"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="67"/>
       <c r="B27" s="67"/>
       <c r="O27" s="68"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="67"/>
       <c r="B28" s="67"/>
       <c r="O28" s="68"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="67"/>
       <c r="B29" s="67"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="67"/>
       <c r="B30" s="67"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="67"/>
       <c r="B31" s="67"/>
     </row>
@@ -11002,12 +11425,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E25:S28 E14:S14 E11:S12 O18:S22 E18:M22 N18:N23">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:W9">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
+      <formula>1996</formula>
+      <formula>2012</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB6:AF24">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>1996</formula>
       <formula>2012</formula>
     </cfRule>
@@ -11021,7 +11450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O34" sqref="O2:O34"/>
     </sheetView>
   </sheetViews>
@@ -11031,7 +11460,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="83" t="s">
         <v>13</v>
       </c>
       <c r="K1" t="s">
@@ -11057,11 +11486,11 @@
         <v xml:space="preserve">   2234  </v>
       </c>
       <c r="M2" t="str">
-        <f>CONCATENATE(quote,G2,quote,comma)</f>
+        <f t="shared" ref="M2:M34" si="0">CONCATENATE(quote,G2,quote,comma)</f>
         <v>"Catholic",</v>
       </c>
       <c r="O2" t="str">
-        <f>CONCATENATE(quote,I2,quote,comma)</f>
+        <f t="shared" ref="O2:O34" si="1">CONCATENATE(quote,I2,quote,comma)</f>
         <v>"Catholic",</v>
       </c>
     </row>
@@ -11070,7 +11499,7 @@
         <v>373</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B34" si="0">MID(A3,21,40)</f>
+        <f t="shared" ref="B3:B34" si="2">MID(A3,21,40)</f>
         <v xml:space="preserve"> Baptist</v>
       </c>
       <c r="G3" t="s">
@@ -11080,15 +11509,15 @@
         <v>438</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K34" si="1">LEFT(A3,9)</f>
+        <f t="shared" ref="K3:K34" si="3">LEFT(A3,9)</f>
         <v xml:space="preserve">    1854 </v>
       </c>
       <c r="M3" t="str">
-        <f>CONCATENATE(quote,G3,quote,comma)</f>
+        <f t="shared" si="0"/>
         <v>"Baptist",</v>
       </c>
       <c r="O3" t="str">
-        <f>CONCATENATE(quote,I3,quote,comma)</f>
+        <f t="shared" si="1"/>
         <v>"Baptic",</v>
       </c>
     </row>
@@ -11097,7 +11526,7 @@
         <v>374</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Methodist</v>
       </c>
       <c r="G4" t="s">
@@ -11107,15 +11536,15 @@
         <v>406</v>
       </c>
       <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     524 </v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Methodist",</v>
+      </c>
+      <c r="O4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     524 </v>
-      </c>
-      <c r="M4" t="str">
-        <f>CONCATENATE(quote,G4,quote,comma)</f>
-        <v>"Methodist",</v>
-      </c>
-      <c r="O4" t="str">
-        <f>CONCATENATE(quote,I4,quote,comma)</f>
         <v>"Methodist",</v>
       </c>
     </row>
@@ -11124,7 +11553,7 @@
         <v>375</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Lutheran</v>
       </c>
       <c r="G5" t="s">
@@ -11134,15 +11563,15 @@
         <v>407</v>
       </c>
       <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     406 </v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Lutheran",</v>
+      </c>
+      <c r="O5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     406 </v>
-      </c>
-      <c r="M5" t="str">
-        <f>CONCATENATE(quote,G5,quote,comma)</f>
-        <v>"Lutheran",</v>
-      </c>
-      <c r="O5" t="str">
-        <f>CONCATENATE(quote,I5,quote,comma)</f>
         <v>"Lutheran",</v>
       </c>
     </row>
@@ -11151,7 +11580,7 @@
         <v>376</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Presbyterian</v>
       </c>
       <c r="G6" t="s">
@@ -11161,15 +11590,15 @@
         <v>408</v>
       </c>
       <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     150 </v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Presbyterian",</v>
+      </c>
+      <c r="O6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     150 </v>
-      </c>
-      <c r="M6" t="str">
-        <f>CONCATENATE(quote,G6,quote,comma)</f>
-        <v>"Presbyterian",</v>
-      </c>
-      <c r="O6" t="str">
-        <f>CONCATENATE(quote,I6,quote,comma)</f>
         <v>"Presbyterian",</v>
       </c>
     </row>
@@ -11178,7 +11607,7 @@
         <v>377</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Episcopal/Anglican</v>
       </c>
       <c r="G7" t="s">
@@ -11188,15 +11617,15 @@
         <v>409</v>
       </c>
       <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     103 </v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Episcopal",</v>
+      </c>
+      <c r="O7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     103 </v>
-      </c>
-      <c r="M7" t="str">
-        <f>CONCATENATE(quote,G7,quote,comma)</f>
-        <v>"Episcopal",</v>
-      </c>
-      <c r="O7" t="str">
-        <f>CONCATENATE(quote,I7,quote,comma)</f>
         <v>"Episcopal",</v>
       </c>
     </row>
@@ -11205,7 +11634,7 @@
         <v>378</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> United Church of Christ (or Congregatio</v>
       </c>
       <c r="G8" t="s">
@@ -11215,15 +11644,15 @@
         <v>416</v>
       </c>
       <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     142 </v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>"C.Christ",</v>
+      </c>
+      <c r="O8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     142 </v>
-      </c>
-      <c r="M8" t="str">
-        <f>CONCATENATE(quote,G8,quote,comma)</f>
-        <v>"C.Christ",</v>
-      </c>
-      <c r="O8" t="str">
-        <f>CONCATENATE(quote,I8,quote,comma)</f>
         <v>"OtherProt",</v>
       </c>
     </row>
@@ -11232,7 +11661,7 @@
         <v>379</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Disciples of Christ (or the Christian C</v>
       </c>
       <c r="G9" t="s">
@@ -11242,15 +11671,15 @@
         <v>416</v>
       </c>
       <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     101 </v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>"D.Christ",</v>
+      </c>
+      <c r="O9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     101 </v>
-      </c>
-      <c r="M9" t="str">
-        <f>CONCATENATE(quote,G9,quote,comma)</f>
-        <v>"D.Christ",</v>
-      </c>
-      <c r="O9" t="str">
-        <f>CONCATENATE(quote,I9,quote,comma)</f>
         <v>"OtherProt",</v>
       </c>
     </row>
@@ -11259,7 +11688,7 @@
         <v>380</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Reform (or Reformed Church in America o</v>
       </c>
       <c r="G10" t="s">
@@ -11269,15 +11698,15 @@
         <v>416</v>
       </c>
       <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      36 </v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Reformed",</v>
+      </c>
+      <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      36 </v>
-      </c>
-      <c r="M10" t="str">
-        <f>CONCATENATE(quote,G10,quote,comma)</f>
-        <v>"Reformed",</v>
-      </c>
-      <c r="O10" t="str">
-        <f>CONCATENATE(quote,I10,quote,comma)</f>
         <v>"OtherProt",</v>
       </c>
     </row>
@@ -11286,7 +11715,7 @@
         <v>381</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Holiness (Nazarene, Wesleyan, Free Met</v>
       </c>
       <c r="G11" t="s">
@@ -11296,15 +11725,15 @@
         <v>416</v>
       </c>
       <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     129 </v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Holiness",</v>
+      </c>
+      <c r="O11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     129 </v>
-      </c>
-      <c r="M11" t="str">
-        <f>CONCATENATE(quote,G11,quote,comma)</f>
-        <v>"Holiness",</v>
-      </c>
-      <c r="O11" t="str">
-        <f>CONCATENATE(quote,I11,quote,comma)</f>
         <v>"OtherProt",</v>
       </c>
     </row>
@@ -11313,7 +11742,7 @@
         <v>382</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Pentecostal (Assembly of God, Pentecos</v>
       </c>
       <c r="G12" t="s">
@@ -11323,15 +11752,15 @@
         <v>414</v>
       </c>
       <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     417 </v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pentecostal",</v>
+      </c>
+      <c r="O12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     417 </v>
-      </c>
-      <c r="M12" t="str">
-        <f>CONCATENATE(quote,G12,quote,comma)</f>
-        <v>"Pentecostal",</v>
-      </c>
-      <c r="O12" t="str">
-        <f>CONCATENATE(quote,I12,quote,comma)</f>
         <v>"Pentecostal",</v>
       </c>
     </row>
@@ -11340,7 +11769,7 @@
         <v>383</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Nondemonimational Christian (Bible Chu</v>
       </c>
       <c r="G13" t="s">
@@ -11350,15 +11779,15 @@
         <v>415</v>
       </c>
       <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     524 </v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Non-Denom",</v>
+      </c>
+      <c r="O13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     524 </v>
-      </c>
-      <c r="M13" t="str">
-        <f>CONCATENATE(quote,G13,quote,comma)</f>
-        <v>"Non-Denom",</v>
-      </c>
-      <c r="O13" t="str">
-        <f>CONCATENATE(quote,I13,quote,comma)</f>
         <v>"Non-Denom",</v>
       </c>
     </row>
@@ -11367,7 +11796,7 @@
         <v>384</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Other Protestant</v>
       </c>
       <c r="G14" t="s">
@@ -11377,15 +11806,15 @@
         <v>416</v>
       </c>
       <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     396 </v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>"OtherProt",</v>
+      </c>
+      <c r="O14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     396 </v>
-      </c>
-      <c r="M14" t="str">
-        <f>CONCATENATE(quote,G14,quote,comma)</f>
-        <v>"OtherProt",</v>
-      </c>
-      <c r="O14" t="str">
-        <f>CONCATENATE(quote,I14,quote,comma)</f>
         <v>"OtherProt",</v>
       </c>
     </row>
@@ -11394,7 +11823,7 @@
         <v>385</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Jewish  -  Orthodox</v>
       </c>
       <c r="G15" t="s">
@@ -11404,15 +11833,15 @@
         <v>439</v>
       </c>
       <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      12 </v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>"JewishOrth",</v>
+      </c>
+      <c r="O15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      12 </v>
-      </c>
-      <c r="M15" t="str">
-        <f>CONCATENATE(quote,G15,quote,comma)</f>
-        <v>"JewishOrth",</v>
-      </c>
-      <c r="O15" t="str">
-        <f>CONCATENATE(quote,I15,quote,comma)</f>
         <v>"Jewish",</v>
       </c>
     </row>
@@ -11421,7 +11850,7 @@
         <v>386</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Jewish  -  Conservative</v>
       </c>
       <c r="G16" t="s">
@@ -11431,15 +11860,15 @@
         <v>439</v>
       </c>
       <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      22 </v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>"JewishCons",</v>
+      </c>
+      <c r="O16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      22 </v>
-      </c>
-      <c r="M16" t="str">
-        <f>CONCATENATE(quote,G16,quote,comma)</f>
-        <v>"JewishCons",</v>
-      </c>
-      <c r="O16" t="str">
-        <f>CONCATENATE(quote,I16,quote,comma)</f>
         <v>"Jewish",</v>
       </c>
     </row>
@@ -11448,7 +11877,7 @@
         <v>387</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Jewish  -  Reform</v>
       </c>
       <c r="G17" t="s">
@@ -11458,15 +11887,15 @@
         <v>439</v>
       </c>
       <c r="K17" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      31 </v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>"JewishRef",</v>
+      </c>
+      <c r="O17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      31 </v>
-      </c>
-      <c r="M17" t="str">
-        <f>CONCATENATE(quote,G17,quote,comma)</f>
-        <v>"JewishRef",</v>
-      </c>
-      <c r="O17" t="str">
-        <f>CONCATENATE(quote,I17,quote,comma)</f>
         <v>"Jewish",</v>
       </c>
     </row>
@@ -11475,7 +11904,7 @@
         <v>388</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Jewish  -  Other Jewish</v>
       </c>
       <c r="G18" t="s">
@@ -11485,15 +11914,15 @@
         <v>439</v>
       </c>
       <c r="K18" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       7 </v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>"JewishOth",</v>
+      </c>
+      <c r="O18" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       7 </v>
-      </c>
-      <c r="M18" t="str">
-        <f>CONCATENATE(quote,G18,quote,comma)</f>
-        <v>"JewishOth",</v>
-      </c>
-      <c r="O18" t="str">
-        <f>CONCATENATE(quote,I18,quote,comma)</f>
         <v>"Jewish",</v>
       </c>
     </row>
@@ -11502,7 +11931,7 @@
         <v>389</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Mormon (all types of Latter Day Saints</v>
       </c>
       <c r="G19" t="s">
@@ -11512,15 +11941,15 @@
         <v>421</v>
       </c>
       <c r="K19" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      92 </v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>"Mormon",</v>
+      </c>
+      <c r="O19" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      92 </v>
-      </c>
-      <c r="M19" t="str">
-        <f>CONCATENATE(quote,G19,quote,comma)</f>
-        <v>"Mormon",</v>
-      </c>
-      <c r="O19" t="str">
-        <f>CONCATENATE(quote,I19,quote,comma)</f>
         <v>"Mormon",</v>
       </c>
     </row>
@@ -11529,7 +11958,7 @@
         <v>390</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Eastern Orthodox</v>
       </c>
       <c r="G20" t="s">
@@ -11539,15 +11968,15 @@
         <v>422</v>
       </c>
       <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      12 </v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="0"/>
+        <v>"EastOrth",</v>
+      </c>
+      <c r="O20" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      12 </v>
-      </c>
-      <c r="M20" t="str">
-        <f>CONCATENATE(quote,G20,quote,comma)</f>
-        <v>"EastOrth",</v>
-      </c>
-      <c r="O20" t="str">
-        <f>CONCATENATE(quote,I20,quote,comma)</f>
         <v>"EastOrth",</v>
       </c>
     </row>
@@ -11556,7 +11985,7 @@
         <v>391</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Unitarian</v>
       </c>
       <c r="G21" t="s">
@@ -11566,15 +11995,15 @@
         <v>423</v>
       </c>
       <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      15 </v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Unitarian",</v>
+      </c>
+      <c r="O21" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      15 </v>
-      </c>
-      <c r="M21" t="str">
-        <f>CONCATENATE(quote,G21,quote,comma)</f>
-        <v>"Unitarian",</v>
-      </c>
-      <c r="O21" t="str">
-        <f>CONCATENATE(quote,I21,quote,comma)</f>
         <v>"Unitarian",</v>
       </c>
     </row>
@@ -11583,7 +12012,7 @@
         <v>392</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Muslim (or Moslem or Islam)</v>
       </c>
       <c r="G22" t="s">
@@ -11593,15 +12022,15 @@
         <v>424</v>
       </c>
       <c r="K22" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      52 </v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Muslim",</v>
+      </c>
+      <c r="O22" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      52 </v>
-      </c>
-      <c r="M22" t="str">
-        <f>CONCATENATE(quote,G22,quote,comma)</f>
-        <v>"Muslim",</v>
-      </c>
-      <c r="O22" t="str">
-        <f>CONCATENATE(quote,I22,quote,comma)</f>
         <v>"Muslim",</v>
       </c>
     </row>
@@ -11610,7 +12039,7 @@
         <v>393</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Hindu/Buddhist</v>
       </c>
       <c r="G23" t="s">
@@ -11620,15 +12049,15 @@
         <v>437</v>
       </c>
       <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      20 </v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Hindu",</v>
+      </c>
+      <c r="O23" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      20 </v>
-      </c>
-      <c r="M23" t="str">
-        <f>CONCATENATE(quote,G23,quote,comma)</f>
-        <v>"Hindu",</v>
-      </c>
-      <c r="O23" t="str">
-        <f>CONCATENATE(quote,I23,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11637,7 +12066,7 @@
         <v>394</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Native American Tribal Religion</v>
       </c>
       <c r="G24" t="s">
@@ -11647,15 +12076,15 @@
         <v>437</v>
       </c>
       <c r="K24" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      17 </v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="0"/>
+        <v>"NATribal",</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      17 </v>
-      </c>
-      <c r="M24" t="str">
-        <f>CONCATENATE(quote,G24,quote,comma)</f>
-        <v>"NATribal",</v>
-      </c>
-      <c r="O24" t="str">
-        <f>CONCATENATE(quote,I24,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11664,7 +12093,7 @@
         <v>430</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  None, no religion - Agnostic (doesn't </v>
       </c>
       <c r="G25" t="s">
@@ -11674,15 +12103,15 @@
         <v>437</v>
       </c>
       <c r="K25" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      90 </v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="0"/>
+        <v>"Agnostic",</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      90 </v>
-      </c>
-      <c r="M25" t="str">
-        <f>CONCATENATE(quote,G25,quote,comma)</f>
-        <v>"Agnostic",</v>
-      </c>
-      <c r="O25" t="str">
-        <f>CONCATENATE(quote,I25,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11701,15 +12130,15 @@
         <v>437</v>
       </c>
       <c r="K26" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      29 </v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="0"/>
+        <v>"Atheist",</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      29 </v>
-      </c>
-      <c r="M26" t="str">
-        <f>CONCATENATE(quote,G26,quote,comma)</f>
-        <v>"Atheist",</v>
-      </c>
-      <c r="O26" t="str">
-        <f>CONCATENATE(quote,I26,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11718,7 +12147,7 @@
         <v>396</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  None, no religion - Personal philosoph</v>
       </c>
       <c r="G27" t="s">
@@ -11728,15 +12157,15 @@
         <v>437</v>
       </c>
       <c r="K27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">     463 </v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="0"/>
+        <v>"PersPhil",</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">     463 </v>
-      </c>
-      <c r="M27" t="str">
-        <f>CONCATENATE(quote,G27,quote,comma)</f>
-        <v>"PersPhil",</v>
-      </c>
-      <c r="O27" t="str">
-        <f>CONCATENATE(quote,I27,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11745,7 +12174,7 @@
         <v>397</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Bah'ai</v>
       </c>
       <c r="G28" t="s">
@@ -11755,15 +12184,15 @@
         <v>437</v>
       </c>
       <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       0 </v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bah'ai",</v>
+      </c>
+      <c r="O28" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       0 </v>
-      </c>
-      <c r="M28" t="str">
-        <f>CONCATENATE(quote,G28,quote,comma)</f>
-        <v>"Bah'ai",</v>
-      </c>
-      <c r="O28" t="str">
-        <f>CONCATENATE(quote,I28,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11772,7 +12201,7 @@
         <v>398</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Greek, Roman, Norse, Etc. Mythology</v>
       </c>
       <c r="G29" t="s">
@@ -11782,15 +12211,15 @@
         <v>437</v>
       </c>
       <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       0 </v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Myth",</v>
+      </c>
+      <c r="O29" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       0 </v>
-      </c>
-      <c r="M29" t="str">
-        <f>CONCATENATE(quote,G29,quote,comma)</f>
-        <v>"Myth",</v>
-      </c>
-      <c r="O29" t="str">
-        <f>CONCATENATE(quote,I29,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11799,7 +12228,7 @@
         <v>399</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Satanic</v>
       </c>
       <c r="G30" t="s">
@@ -11809,15 +12238,15 @@
         <v>437</v>
       </c>
       <c r="K30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       1 </v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Satanic",</v>
+      </c>
+      <c r="O30" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       1 </v>
-      </c>
-      <c r="M30" t="str">
-        <f>CONCATENATE(quote,G30,quote,comma)</f>
-        <v>"Satanic",</v>
-      </c>
-      <c r="O30" t="str">
-        <f>CONCATENATE(quote,I30,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11826,7 +12255,7 @@
         <v>400</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Wicca/Witchcraft/Magic/Pagan</v>
       </c>
       <c r="G31" t="s">
@@ -11836,15 +12265,15 @@
         <v>437</v>
       </c>
       <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       8 </v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="0"/>
+        <v>"Witchcraft",</v>
+      </c>
+      <c r="O31" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       8 </v>
-      </c>
-      <c r="M31" t="str">
-        <f>CONCATENATE(quote,G31,quote,comma)</f>
-        <v>"Witchcraft",</v>
-      </c>
-      <c r="O31" t="str">
-        <f>CONCATENATE(quote,I31,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11853,7 +12282,7 @@
         <v>401</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Scientology</v>
       </c>
       <c r="G32" t="s">
@@ -11863,15 +12292,15 @@
         <v>437</v>
       </c>
       <c r="K32" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       1 </v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="0"/>
+        <v>"Scientology",</v>
+      </c>
+      <c r="O32" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       1 </v>
-      </c>
-      <c r="M32" t="str">
-        <f>CONCATENATE(quote,G32,quote,comma)</f>
-        <v>"Scientology",</v>
-      </c>
-      <c r="O32" t="str">
-        <f>CONCATENATE(quote,I32,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>
@@ -11880,7 +12309,7 @@
         <v>402</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Other Eastern (Sikh)</v>
       </c>
       <c r="G33" t="s">
@@ -11890,15 +12319,15 @@
         <v>436</v>
       </c>
       <c r="K33" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">       2 </v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="0"/>
+        <v>"Sikh",</v>
+      </c>
+      <c r="O33" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">       2 </v>
-      </c>
-      <c r="M33" t="str">
-        <f>CONCATENATE(quote,G33,quote,comma)</f>
-        <v>"Sikh",</v>
-      </c>
-      <c r="O33" t="str">
-        <f>CONCATENATE(quote,I33,quote,comma)</f>
         <v>"Sikh",</v>
       </c>
     </row>
@@ -11907,7 +12336,7 @@
         <v>403</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  Other (SPECIFY)</v>
       </c>
       <c r="G34" t="s">
@@ -11917,15 +12346,15 @@
         <v>437</v>
       </c>
       <c r="K34" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">      24 </v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="0"/>
+        <v>"Other",</v>
+      </c>
+      <c r="O34" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">      24 </v>
-      </c>
-      <c r="M34" t="str">
-        <f>CONCATENATE(quote,G34,quote,comma)</f>
-        <v>"Other",</v>
-      </c>
-      <c r="O34" t="str">
-        <f>CONCATENATE(quote,I34,quote,comma)</f>
         <v>"Other",</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates on readmes and xlsx
</commit_message>
<xml_diff>
--- a/Data/ItemMap_20042014.xlsx
+++ b/Data/ItemMap_20042014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="5"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="18345" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="8" r:id="rId1"/>
@@ -2075,7 +2075,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2170,6 +2170,13 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2215,7 +2222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2357,12 +2364,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2604,9 +2633,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2628,20 +2654,544 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
@@ -2816,44 +3366,6 @@
     </dxf>
     <dxf>
       <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="2"/>
         </patternFill>
@@ -2862,7 +3374,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3220,8 +3732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,26 +3782,26 @@
       <c r="B2" s="25" t="s">
         <v>338</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="104" t="s">
         <v>339</v>
       </c>
-      <c r="D2" s="90">
+      <c r="D2" s="89">
         <v>1997</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="92"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="91"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="X2" s="1"/>
@@ -3301,26 +3813,26 @@
       <c r="B3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="90">
+      <c r="D3" s="89">
         <v>1997</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="94"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="X3" s="1"/>
@@ -3332,26 +3844,26 @@
       <c r="B4" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="89">
         <v>1997</v>
       </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="94"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="93"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="X4" s="1"/>
@@ -3363,26 +3875,26 @@
       <c r="B5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="90">
+      <c r="D5" s="89">
         <v>1997</v>
       </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="94"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="93"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="X5" s="1"/>
@@ -3394,26 +3906,26 @@
       <c r="B6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="89">
         <v>1997</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="94"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="92"/>
+      <c r="O6" s="92"/>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="92"/>
+      <c r="R6" s="93"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="X6" s="1"/>
@@ -3425,26 +3937,26 @@
       <c r="B7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="90">
+      <c r="D7" s="89">
         <v>1997</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="96"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="93"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="X7" s="1"/>
@@ -3456,26 +3968,26 @@
       <c r="B8" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="90">
+      <c r="D8" s="89">
         <v>1997</v>
       </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="79"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="91"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="X8" s="1"/>
@@ -3487,26 +3999,26 @@
       <c r="B9" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="105" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="90">
+      <c r="D9" s="89">
         <v>1997</v>
       </c>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="79"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="92"/>
+      <c r="Q9" s="92"/>
+      <c r="R9" s="93"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="X9" s="1"/>
@@ -3518,26 +4030,26 @@
       <c r="B10" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="90">
+      <c r="D10" s="102">
         <v>1997</v>
       </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="97"/>
-      <c r="O10" s="97"/>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="98"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="94"/>
+      <c r="O10" s="94"/>
+      <c r="P10" s="94"/>
+      <c r="Q10" s="94"/>
+      <c r="R10" s="95"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="X10" s="1"/>
@@ -3549,52 +4061,52 @@
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="90">
+      <c r="D11" s="96">
         <v>1997</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="96">
         <v>1998</v>
       </c>
-      <c r="F11" s="93">
+      <c r="F11" s="96">
         <v>1999</v>
       </c>
-      <c r="G11" s="90">
+      <c r="G11" s="96">
         <v>2000</v>
       </c>
-      <c r="H11" s="93">
+      <c r="H11" s="96">
         <v>2001</v>
       </c>
-      <c r="I11" s="93">
+      <c r="I11" s="96">
         <v>2002</v>
       </c>
-      <c r="J11" s="90">
+      <c r="J11" s="96">
         <v>2003</v>
       </c>
-      <c r="K11" s="93">
+      <c r="K11" s="96">
         <v>2004</v>
       </c>
-      <c r="L11" s="93">
+      <c r="L11" s="96">
         <v>2005</v>
       </c>
-      <c r="M11" s="90">
+      <c r="M11" s="96">
         <v>2006</v>
       </c>
-      <c r="N11" s="93">
+      <c r="N11" s="96">
         <v>2007</v>
       </c>
-      <c r="O11" s="93">
+      <c r="O11" s="96">
         <v>2008</v>
       </c>
-      <c r="P11" s="90">
+      <c r="P11" s="96">
         <v>2009</v>
       </c>
-      <c r="Q11" s="93">
+      <c r="Q11" s="96">
         <v>2010</v>
       </c>
-      <c r="R11" s="93">
+      <c r="R11" s="99">
         <v>2011</v>
       </c>
       <c r="S11" s="1"/>
@@ -3608,52 +4120,52 @@
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="90">
+      <c r="D12" s="89">
         <v>1997</v>
       </c>
-      <c r="E12" s="93">
+      <c r="E12" s="89">
         <v>1998</v>
       </c>
-      <c r="F12" s="93">
+      <c r="F12" s="89">
         <v>1999</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="89">
         <v>2000</v>
       </c>
-      <c r="H12" s="93">
+      <c r="H12" s="89">
         <v>2001</v>
       </c>
-      <c r="I12" s="93">
+      <c r="I12" s="89">
         <v>2002</v>
       </c>
-      <c r="J12" s="90">
+      <c r="J12" s="89">
         <v>2003</v>
       </c>
-      <c r="K12" s="93">
+      <c r="K12" s="89">
         <v>2004</v>
       </c>
-      <c r="L12" s="93">
+      <c r="L12" s="89">
         <v>2005</v>
       </c>
-      <c r="M12" s="90">
+      <c r="M12" s="89">
         <v>2006</v>
       </c>
-      <c r="N12" s="93">
+      <c r="N12" s="89">
         <v>2007</v>
       </c>
-      <c r="O12" s="93">
+      <c r="O12" s="89">
         <v>2008</v>
       </c>
-      <c r="P12" s="90">
+      <c r="P12" s="89">
         <v>2009</v>
       </c>
-      <c r="Q12" s="93">
+      <c r="Q12" s="89">
         <v>2010</v>
       </c>
-      <c r="R12" s="93">
+      <c r="R12" s="100">
         <v>2011</v>
       </c>
       <c r="S12" s="1"/>
@@ -3667,32 +4179,32 @@
       <c r="B13" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="90">
+      <c r="D13" s="89">
         <v>1997</v>
       </c>
-      <c r="E13" s="93">
+      <c r="E13" s="89">
         <v>1998</v>
       </c>
-      <c r="F13" s="93">
+      <c r="F13" s="89">
         <v>1999</v>
       </c>
-      <c r="G13" s="90">
+      <c r="G13" s="89">
         <v>2000</v>
       </c>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="91"/>
-      <c r="N13" s="91"/>
-      <c r="O13" s="91"/>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="91"/>
-      <c r="R13" s="92"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="100"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="X13" s="1"/>
@@ -3704,43 +4216,43 @@
       <c r="B14" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="99"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="90">
+      <c r="D14" s="96"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="89">
         <v>2000</v>
       </c>
-      <c r="H14" s="93">
+      <c r="H14" s="92">
         <v>2001</v>
       </c>
-      <c r="I14" s="93">
+      <c r="I14" s="92">
         <v>2002</v>
       </c>
-      <c r="J14" s="90">
+      <c r="J14" s="89">
         <v>2003</v>
       </c>
-      <c r="K14" s="93">
+      <c r="K14" s="92">
         <v>2004</v>
       </c>
-      <c r="L14" s="93">
+      <c r="L14" s="92">
         <v>2005</v>
       </c>
-      <c r="M14" s="90">
+      <c r="M14" s="89">
         <v>2006</v>
       </c>
-      <c r="N14" s="93">
+      <c r="N14" s="92">
         <v>2007</v>
       </c>
-      <c r="O14" s="93">
+      <c r="O14" s="92">
         <v>2008</v>
       </c>
-      <c r="P14" s="90">
+      <c r="P14" s="89">
         <v>2009</v>
       </c>
-      <c r="Q14" s="93">
+      <c r="Q14" s="92">
         <v>2010</v>
       </c>
       <c r="R14" s="93">
@@ -3757,30 +4269,30 @@
       <c r="B15" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93">
+      <c r="D15" s="96"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="90">
         <v>2002</v>
       </c>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93">
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="90">
         <v>2005</v>
       </c>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="93">
+      <c r="M15" s="92"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="89">
         <v>2008</v>
       </c>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93">
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="100">
         <v>2011</v>
       </c>
       <c r="S15" s="1"/>
@@ -3794,30 +4306,30 @@
       <c r="B16" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93">
+      <c r="D16" s="96"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="90">
         <v>2002</v>
       </c>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93">
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="90">
         <v>2005</v>
       </c>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93">
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="89">
         <v>2008</v>
       </c>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93">
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="100">
         <v>2011</v>
       </c>
       <c r="S16" s="1"/>
@@ -3831,30 +4343,30 @@
       <c r="B17" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="99"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93">
+      <c r="D17" s="96"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="90">
         <v>2002</v>
       </c>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93">
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="90">
         <v>2005</v>
       </c>
-      <c r="M17" s="93"/>
-      <c r="N17" s="93"/>
-      <c r="O17" s="93">
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="89">
         <v>2008</v>
       </c>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="93"/>
-      <c r="R17" s="93">
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
+      <c r="R17" s="100">
         <v>2011</v>
       </c>
       <c r="S17" s="1"/>
@@ -3868,30 +4380,30 @@
       <c r="B18" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93">
+      <c r="D18" s="96"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="90">
         <v>2002</v>
       </c>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93">
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="90">
         <v>2005</v>
       </c>
-      <c r="M18" s="93"/>
-      <c r="N18" s="93"/>
-      <c r="O18" s="93">
+      <c r="M18" s="92"/>
+      <c r="N18" s="92"/>
+      <c r="O18" s="89">
         <v>2008</v>
       </c>
-      <c r="P18" s="93"/>
-      <c r="Q18" s="93"/>
-      <c r="R18" s="93">
+      <c r="P18" s="92"/>
+      <c r="Q18" s="92"/>
+      <c r="R18" s="100">
         <v>2011</v>
       </c>
       <c r="S18" s="1"/>
@@ -3905,30 +4417,30 @@
       <c r="B19" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="99"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93">
+      <c r="D19" s="96"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="90">
         <v>2002</v>
       </c>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93">
+      <c r="J19" s="92"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="90">
         <v>2005</v>
       </c>
-      <c r="M19" s="93"/>
-      <c r="N19" s="93"/>
-      <c r="O19" s="93">
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="89">
         <v>2008</v>
       </c>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="93"/>
-      <c r="R19" s="93">
+      <c r="P19" s="92"/>
+      <c r="Q19" s="92"/>
+      <c r="R19" s="100">
         <v>2011</v>
       </c>
       <c r="S19" s="1"/>
@@ -3942,28 +4454,28 @@
       <c r="B20" s="47" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="99"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93">
+      <c r="D20" s="96"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="90">
         <v>2005</v>
       </c>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="93">
+      <c r="M20" s="92"/>
+      <c r="N20" s="92"/>
+      <c r="O20" s="89">
         <v>2008</v>
       </c>
-      <c r="P20" s="93"/>
-      <c r="Q20" s="93"/>
-      <c r="R20" s="93">
+      <c r="P20" s="92"/>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="100">
         <v>2011</v>
       </c>
       <c r="S20" s="1"/>
@@ -3977,26 +4489,26 @@
       <c r="B21" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="99"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93">
+      <c r="D21" s="96"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="92"/>
+      <c r="M21" s="92"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="90">
         <v>2008</v>
       </c>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
-      <c r="R21" s="93">
+      <c r="P21" s="92"/>
+      <c r="Q21" s="92"/>
+      <c r="R21" s="100">
         <v>2011</v>
       </c>
       <c r="S21" s="1"/>
@@ -4010,26 +4522,26 @@
       <c r="B22" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="100"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="95"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="93">
+      <c r="D22" s="96"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="90">
         <v>2008</v>
       </c>
-      <c r="P22" s="95"/>
-      <c r="Q22" s="95"/>
-      <c r="R22" s="93">
+      <c r="P22" s="92"/>
+      <c r="Q22" s="92"/>
+      <c r="R22" s="100">
         <v>2011</v>
       </c>
       <c r="S22" s="1"/>
@@ -4043,36 +4555,36 @@
       <c r="B23" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="107" t="s">
         <v>340</v>
       </c>
-      <c r="D23" s="90"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="90">
         <v>2000</v>
       </c>
-      <c r="H23" s="75"/>
-      <c r="I23" s="93">
+      <c r="H23" s="90"/>
+      <c r="I23" s="90">
         <v>2002</v>
       </c>
-      <c r="J23" s="75"/>
-      <c r="K23" s="93">
+      <c r="J23" s="90"/>
+      <c r="K23" s="89">
         <v>2004</v>
       </c>
-      <c r="L23" s="75"/>
-      <c r="M23" s="90">
+      <c r="L23" s="89"/>
+      <c r="M23" s="89">
         <v>2006</v>
       </c>
-      <c r="N23" s="75"/>
-      <c r="O23" s="93">
+      <c r="N23" s="90"/>
+      <c r="O23" s="89">
         <v>2008</v>
       </c>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="93">
+      <c r="P23" s="90"/>
+      <c r="Q23" s="89">
         <v>2010</v>
       </c>
-      <c r="R23" s="76"/>
+      <c r="R23" s="91"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="X23" s="1"/>
@@ -4084,36 +4596,36 @@
       <c r="B24" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
       <c r="G24" s="90">
         <v>2000</v>
       </c>
-      <c r="H24" s="78"/>
-      <c r="I24" s="93">
+      <c r="H24" s="92"/>
+      <c r="I24" s="90">
         <v>2002</v>
       </c>
-      <c r="J24" s="78"/>
-      <c r="K24" s="93">
+      <c r="J24" s="92"/>
+      <c r="K24" s="89">
         <v>2004</v>
       </c>
-      <c r="L24" s="78"/>
-      <c r="M24" s="90">
+      <c r="L24" s="92"/>
+      <c r="M24" s="89">
         <v>2006</v>
       </c>
-      <c r="N24" s="78"/>
-      <c r="O24" s="93">
+      <c r="N24" s="92"/>
+      <c r="O24" s="89">
         <v>2008</v>
       </c>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="93">
+      <c r="P24" s="92"/>
+      <c r="Q24" s="89">
         <v>2010</v>
       </c>
-      <c r="R24" s="79"/>
+      <c r="R24" s="93"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="X24" s="1"/>
@@ -4125,36 +4637,36 @@
       <c r="B25" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
       <c r="G25" s="90">
         <v>2000</v>
       </c>
-      <c r="H25" s="78"/>
-      <c r="I25" s="93">
+      <c r="H25" s="92"/>
+      <c r="I25" s="90">
         <v>2002</v>
       </c>
-      <c r="J25" s="78"/>
-      <c r="K25" s="93">
+      <c r="J25" s="92"/>
+      <c r="K25" s="89">
         <v>2004</v>
       </c>
-      <c r="L25" s="78"/>
-      <c r="M25" s="90">
+      <c r="L25" s="92"/>
+      <c r="M25" s="89">
         <v>2006</v>
       </c>
-      <c r="N25" s="78"/>
-      <c r="O25" s="93">
+      <c r="N25" s="92"/>
+      <c r="O25" s="89">
         <v>2008</v>
       </c>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="93">
+      <c r="P25" s="92"/>
+      <c r="Q25" s="89">
         <v>2010</v>
       </c>
-      <c r="R25" s="79"/>
+      <c r="R25" s="93"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="X25" s="1"/>
@@ -4166,36 +4678,36 @@
       <c r="B26" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
       <c r="G26" s="90">
         <v>2000</v>
       </c>
-      <c r="H26" s="78"/>
-      <c r="I26" s="93">
+      <c r="H26" s="92"/>
+      <c r="I26" s="90">
         <v>2002</v>
       </c>
-      <c r="J26" s="78"/>
-      <c r="K26" s="93">
+      <c r="J26" s="92"/>
+      <c r="K26" s="89">
         <v>2004</v>
       </c>
-      <c r="L26" s="78"/>
-      <c r="M26" s="90">
+      <c r="L26" s="92"/>
+      <c r="M26" s="89">
         <v>2006</v>
       </c>
-      <c r="N26" s="78"/>
-      <c r="O26" s="93">
+      <c r="N26" s="92"/>
+      <c r="O26" s="89">
         <v>2008</v>
       </c>
-      <c r="P26" s="78"/>
-      <c r="Q26" s="93">
+      <c r="P26" s="92"/>
+      <c r="Q26" s="89">
         <v>2010</v>
       </c>
-      <c r="R26" s="79"/>
+      <c r="R26" s="93"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="X26" s="1"/>
@@ -4207,36 +4719,36 @@
       <c r="B27" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="90">
+      <c r="D27" s="97"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="101">
         <v>2000</v>
       </c>
-      <c r="H27" s="81"/>
-      <c r="I27" s="93">
+      <c r="H27" s="94"/>
+      <c r="I27" s="101">
         <v>2002</v>
       </c>
-      <c r="J27" s="81"/>
-      <c r="K27" s="93">
+      <c r="J27" s="94"/>
+      <c r="K27" s="102">
         <v>2004</v>
       </c>
-      <c r="L27" s="81"/>
-      <c r="M27" s="90">
+      <c r="L27" s="94"/>
+      <c r="M27" s="102">
         <v>2006</v>
       </c>
-      <c r="N27" s="81"/>
-      <c r="O27" s="93">
+      <c r="N27" s="94"/>
+      <c r="O27" s="102">
         <v>2008</v>
       </c>
-      <c r="P27" s="81"/>
-      <c r="Q27" s="93">
+      <c r="P27" s="94"/>
+      <c r="Q27" s="102">
         <v>2010</v>
       </c>
-      <c r="R27" s="82"/>
+      <c r="R27" s="95"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="X27" s="1"/>
@@ -4248,34 +4760,34 @@
       <c r="B28" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="93">
+      <c r="D28" s="89"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90">
         <v>2002</v>
       </c>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="93">
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="89">
         <v>2007</v>
       </c>
-      <c r="O28" s="93">
+      <c r="O28" s="89">
         <v>2008</v>
       </c>
-      <c r="P28" s="90">
+      <c r="P28" s="89">
         <v>2009</v>
       </c>
-      <c r="Q28" s="93">
+      <c r="Q28" s="89">
         <v>2010</v>
       </c>
-      <c r="R28" s="93">
+      <c r="R28" s="100">
         <v>2011</v>
       </c>
       <c r="S28" s="1"/>
@@ -4289,34 +4801,34 @@
       <c r="B29" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="77"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="93">
+      <c r="D29" s="96"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="90">
         <v>2002</v>
       </c>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="93">
+      <c r="J29" s="92"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="92"/>
+      <c r="N29" s="89">
         <v>2007</v>
       </c>
-      <c r="O29" s="93">
+      <c r="O29" s="89">
         <v>2008</v>
       </c>
-      <c r="P29" s="90">
+      <c r="P29" s="89">
         <v>2009</v>
       </c>
-      <c r="Q29" s="93">
+      <c r="Q29" s="89">
         <v>2010</v>
       </c>
-      <c r="R29" s="93">
+      <c r="R29" s="100">
         <v>2011</v>
       </c>
       <c r="S29" s="1"/>
@@ -4330,42 +4842,42 @@
       <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="100"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="93">
+      <c r="D30" s="97"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="101">
         <v>2002</v>
       </c>
-      <c r="J30" s="90">
+      <c r="J30" s="102">
         <v>2003</v>
       </c>
-      <c r="K30" s="93">
+      <c r="K30" s="102">
         <v>2004</v>
       </c>
-      <c r="L30" s="90">
+      <c r="L30" s="102">
         <v>2005</v>
       </c>
-      <c r="M30" s="93">
+      <c r="M30" s="102">
         <v>2006</v>
       </c>
-      <c r="N30" s="90">
+      <c r="N30" s="102">
         <v>2007</v>
       </c>
-      <c r="O30" s="93">
+      <c r="O30" s="102">
         <v>2008</v>
       </c>
-      <c r="P30" s="90">
+      <c r="P30" s="102">
         <v>2009</v>
       </c>
-      <c r="Q30" s="93">
+      <c r="Q30" s="102">
         <v>2010</v>
       </c>
-      <c r="R30" s="90">
+      <c r="R30" s="103">
         <v>2011</v>
       </c>
       <c r="S30" s="1"/>
@@ -4540,12 +5052,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D54:R57 D34:R34 D43:R43 B11:C12 B14:C14 D40:R41 N47:R51 D47:L51 M47:M52">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:R30">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+  <conditionalFormatting sqref="G14:R14">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="between">
+      <formula>1997</formula>
+      <formula>2011</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:R13">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="between">
+      <formula>1997</formula>
+      <formula>2011</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:R30">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
       <formula>1997</formula>
       <formula>2011</formula>
     </cfRule>
@@ -7369,12 +7893,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="98" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="64" t="s">
         <v>368</v>
       </c>
@@ -11206,18 +11730,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E25:S28 E14:S14 E11:S12 O18:S22 E18:M22 N18:N23">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:W9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="between">
       <formula>1996</formula>
       <formula>2012</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6:AF24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="between">
       <formula>1996</formula>
       <formula>2012</formula>
     </cfRule>
@@ -11231,7 +11755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -14558,12 +15082,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D54:R57 D34:R34 D43:R43 B11:C12 B14:C14 D40:R41 N47:R51 D47:L51 M47:M52">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:R30">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16915,12 +17439,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D53:R56 M42:M51 D33:R33 D42:L50 N42:R50 B8:C9 B11:C11 D37:R40">
-    <cfRule type="containsText" dxfId="5" priority="70" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="22" priority="70" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:R31">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated figures in Extract
</commit_message>
<xml_diff>
--- a/Data/ItemMap_20042014.xlsx
+++ b/Data/ItemMap_20042014.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="448">
   <si>
     <t>x</t>
   </si>
@@ -2087,6 +2087,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 1/0</t>
+  </si>
+  <si>
+    <t># days</t>
   </si>
 </sst>
 </file>
@@ -2721,14 +2724,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2736,11 +2739,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3412,7 +3415,7 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,7 +3461,7 @@
       <c r="A2" s="41" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="112" t="s">
         <v>446</v>
       </c>
       <c r="C2" s="103" t="s">
@@ -3856,7 +3859,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>23</v>
+        <v>447</v>
       </c>
       <c r="C13" s="104" t="s">
         <v>262</v>
@@ -3892,7 +3895,7 @@
       <c r="A14" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="116" t="s">
+      <c r="B14" s="111" t="s">
         <v>444</v>
       </c>
       <c r="C14" s="104" t="s">
@@ -4758,6 +4761,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7572,12 +7578,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="113" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
       <c r="E1" s="64" t="s">
         <v>368</v>
       </c>
@@ -11495,10 +11501,10 @@
       </c>
       <c r="AG32" s="108"/>
       <c r="AH32" s="108"/>
-      <c r="AJ32" s="112">
+      <c r="AJ32" s="116">
         <v>1998</v>
       </c>
-      <c r="AK32" s="113"/>
+      <c r="AK32" s="117"/>
       <c r="AL32" s="77">
         <v>18</v>
       </c>
@@ -11534,10 +11540,10 @@
       </c>
       <c r="AG33" s="108"/>
       <c r="AH33" s="108"/>
-      <c r="AJ33" s="112">
+      <c r="AJ33" s="116">
         <v>1999</v>
       </c>
-      <c r="AK33" s="113"/>
+      <c r="AK33" s="117"/>
       <c r="AL33" s="77">
         <v>19</v>
       </c>
@@ -11575,10 +11581,10 @@
       </c>
       <c r="AG34" s="108"/>
       <c r="AH34" s="108"/>
-      <c r="AJ34" s="112">
+      <c r="AJ34" s="116">
         <v>2000</v>
       </c>
-      <c r="AK34" s="113"/>
+      <c r="AK34" s="117"/>
       <c r="AL34" s="77">
         <v>20</v>
       </c>
@@ -11618,10 +11624,10 @@
       </c>
       <c r="AG35" s="108"/>
       <c r="AH35" s="108"/>
-      <c r="AJ35" s="112">
+      <c r="AJ35" s="116">
         <v>2001</v>
       </c>
-      <c r="AK35" s="113"/>
+      <c r="AK35" s="117"/>
       <c r="AL35" s="77">
         <v>21</v>
       </c>
@@ -11661,10 +11667,10 @@
       </c>
       <c r="AG36" s="108"/>
       <c r="AH36" s="108"/>
-      <c r="AJ36" s="112">
+      <c r="AJ36" s="116">
         <v>2002</v>
       </c>
-      <c r="AK36" s="113"/>
+      <c r="AK36" s="117"/>
       <c r="AL36" s="77">
         <v>22</v>
       </c>
@@ -11702,10 +11708,10 @@
       </c>
       <c r="AG37" s="108"/>
       <c r="AH37" s="108"/>
-      <c r="AJ37" s="112">
+      <c r="AJ37" s="116">
         <v>2003</v>
       </c>
-      <c r="AK37" s="113"/>
+      <c r="AK37" s="117"/>
       <c r="AL37" s="77">
         <v>23</v>
       </c>
@@ -11743,10 +11749,10 @@
       </c>
       <c r="AG38" s="108"/>
       <c r="AH38" s="108"/>
-      <c r="AJ38" s="112">
+      <c r="AJ38" s="116">
         <v>2004</v>
       </c>
-      <c r="AK38" s="113"/>
+      <c r="AK38" s="117"/>
       <c r="AL38" s="77">
         <v>24</v>
       </c>
@@ -11784,10 +11790,10 @@
       </c>
       <c r="AG39" s="108"/>
       <c r="AH39" s="108"/>
-      <c r="AJ39" s="112">
+      <c r="AJ39" s="116">
         <v>2005</v>
       </c>
-      <c r="AK39" s="113"/>
+      <c r="AK39" s="117"/>
       <c r="AL39" s="77">
         <v>25</v>
       </c>
@@ -11825,10 +11831,10 @@
       </c>
       <c r="AG40" s="108"/>
       <c r="AH40" s="108"/>
-      <c r="AJ40" s="112">
+      <c r="AJ40" s="116">
         <v>2006</v>
       </c>
-      <c r="AK40" s="113"/>
+      <c r="AK40" s="117"/>
       <c r="AL40" s="77">
         <v>26</v>
       </c>
@@ -11866,10 +11872,10 @@
       </c>
       <c r="AG41" s="108"/>
       <c r="AH41" s="108"/>
-      <c r="AJ41" s="112">
+      <c r="AJ41" s="116">
         <v>2007</v>
       </c>
-      <c r="AK41" s="113"/>
+      <c r="AK41" s="117"/>
       <c r="AL41" s="77">
         <v>27</v>
       </c>
@@ -11907,10 +11913,10 @@
       </c>
       <c r="AG42" s="108"/>
       <c r="AH42" s="108"/>
-      <c r="AJ42" s="112">
+      <c r="AJ42" s="116">
         <v>2008</v>
       </c>
-      <c r="AK42" s="113"/>
+      <c r="AK42" s="117"/>
       <c r="AL42" s="77">
         <v>28</v>
       </c>
@@ -11948,10 +11954,10 @@
       </c>
       <c r="AG43" s="108"/>
       <c r="AH43" s="108"/>
-      <c r="AJ43" s="112">
+      <c r="AJ43" s="116">
         <v>2009</v>
       </c>
-      <c r="AK43" s="113"/>
+      <c r="AK43" s="117"/>
       <c r="AL43" s="77">
         <v>29</v>
       </c>
@@ -11989,10 +11995,10 @@
       </c>
       <c r="AG44" s="108"/>
       <c r="AH44" s="108"/>
-      <c r="AJ44" s="112">
+      <c r="AJ44" s="116">
         <v>2010</v>
       </c>
-      <c r="AK44" s="113"/>
+      <c r="AK44" s="117"/>
       <c r="AL44" s="77">
         <v>30</v>
       </c>
@@ -12032,10 +12038,10 @@
         <v>443</v>
       </c>
       <c r="AH45" s="108"/>
-      <c r="AJ45" s="112">
+      <c r="AJ45" s="116">
         <v>2011</v>
       </c>
-      <c r="AK45" s="113"/>
+      <c r="AK45" s="117"/>
       <c r="AL45" s="77">
         <v>31</v>
       </c>

</xml_diff>